<commit_message>
BSIS-1281: Add new columns to Location for DataImport Added isProcessingSite, isDistributionSite and isTestingSite to the BSIS Data Importer.
</commit_message>
<xml_diff>
--- a/src/test/resources/fixtures/BSIS-import.xlsx
+++ b/src/test/resources/fixtures/BSIS-import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="975" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="975" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="134">
   <si>
     <t>name</t>
   </si>
@@ -33,6 +33,15 @@
     <t>isVenue</t>
   </si>
   <si>
+    <t>isProcessingSite</t>
+  </si>
+  <si>
+    <t>isDistributionSite</t>
+  </si>
+  <si>
+    <t>isTestingSite</t>
+  </si>
+  <si>
     <t>isDeleted</t>
   </si>
   <si>
@@ -54,7 +63,7 @@
     <t>Fourth</t>
   </si>
   <si>
-    <t>Second venue</t>
+    <t>A venue</t>
   </si>
   <si>
     <t>externalDonorId</t>
@@ -495,12 +504,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -549,10 +562,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -561,9 +574,12 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.4744897959184"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1479591836735"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="55.3469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6785714285714"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="55.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.4234693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -585,10 +601,19 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" s="0" t="n">
         <f aca="false">FALSE()</f>
@@ -602,17 +627,29 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>7</v>
+      <c r="F2" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">FALSE()</f>
@@ -622,18 +659,30 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="2" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="F3" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">TRUE()</f>
@@ -643,18 +692,30 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="2" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B5" s="0" t="n">
         <f aca="false">FALSE()</f>
@@ -668,17 +729,29 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>11</v>
+      <c r="F5" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B1:E1" type="none">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B1:H1" type="none">
       <formula1>booleans</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -717,7 +790,7 @@
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.1479591836735"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.50510204081633"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="3" width="29.4285714285714"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.72959183673469"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.1887755102041"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.8469387755102"/>
@@ -756,139 +829,139 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>5</v>
+        <v>25</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
@@ -898,133 +971,133 @@
         <v>123</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="I2" s="4" t="n">
+        <v>65</v>
+      </c>
+      <c r="I2" s="5" t="n">
         <v>30288</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="O2" s="0" t="n">
         <v>8212030162083</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="Z2" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AB2" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="AC2" s="0" t="n">
         <v>8001</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AD2" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="AF2" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG2" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="AE2" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="AF2" s="0" t="s">
+      <c r="AH2" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="AI2" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="AG2" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="AH2" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="AI2" s="0" t="s">
-        <v>78</v>
-      </c>
       <c r="AJ2" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AK2" s="0" t="n">
         <v>8001</v>
       </c>
       <c r="AL2" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="AM2" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="AN2" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="AO2" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AP2" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="AQ2" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="AR2" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AS2" s="0" t="n">
         <v>8018</v>
@@ -1035,133 +1108,133 @@
         <v>456</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="I3" s="4" t="n">
+        <v>94</v>
+      </c>
+      <c r="I3" s="5" t="n">
         <v>26575</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="O3" s="0" t="n">
         <v>7210030162086</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="Y3" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="Z3" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="AA3" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AB3" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="AC3" s="0" t="n">
         <v>8001</v>
       </c>
-      <c r="AD3" s="5" t="s">
+      <c r="AD3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE3" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="AF3" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG3" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="AE3" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="AF3" s="0" t="s">
+      <c r="AH3" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="AI3" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="AG3" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="AH3" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="AI3" s="0" t="s">
-        <v>78</v>
-      </c>
       <c r="AJ3" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AK3" s="0" t="n">
         <v>8001</v>
       </c>
       <c r="AL3" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="AM3" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="AN3" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="AO3" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AP3" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="AQ3" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="AR3" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AS3" s="0" t="n">
         <v>8018</v>
@@ -1172,29 +1245,29 @@
         <v>789</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D4" s="0" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
       <c r="E4" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F4" s="0" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
       <c r="G4" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="I4" s="6" t="n">
+        <v>65</v>
+      </c>
+      <c r="I4" s="7" t="n">
         <v>36443</v>
       </c>
       <c r="J4" s="0" t="str">
@@ -1207,7 +1280,7 @@
       </c>
       <c r="L4" s="0"/>
       <c r="M4" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N4" s="0" t="str">
         <f aca="false">""</f>
@@ -1356,7 +1429,7 @@
   </sheetPr>
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -1386,61 +1459,61 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1451,21 +1524,21 @@
         <v>3243400</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="F2" s="6" t="n">
+        <v>115</v>
+      </c>
+      <c r="F2" s="7" t="n">
         <v>42432.0833333333</v>
       </c>
-      <c r="G2" s="7" t="n">
+      <c r="G2" s="8" t="n">
         <v>42432.375</v>
       </c>
-      <c r="H2" s="7" t="n">
+      <c r="H2" s="8" t="n">
         <v>42432.38125</v>
       </c>
       <c r="I2" s="0" t="n">
@@ -1484,22 +1557,22 @@
         <v>23</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1510,21 +1583,21 @@
         <v>3243500</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="F3" s="6" t="n">
+        <v>115</v>
+      </c>
+      <c r="F3" s="7" t="n">
         <v>42432.5</v>
       </c>
-      <c r="G3" s="7" t="n">
+      <c r="G3" s="8" t="n">
         <v>42432.3819444444</v>
       </c>
-      <c r="H3" s="7" t="n">
+      <c r="H3" s="8" t="n">
         <v>42432.3840277778</v>
       </c>
       <c r="I3" s="0" t="n">
@@ -1543,22 +1616,22 @@
         <v>23</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1569,21 +1642,21 @@
         <v>3243200</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="F4" s="6" t="n">
+        <v>115</v>
+      </c>
+      <c r="F4" s="7" t="n">
         <v>42372</v>
       </c>
-      <c r="G4" s="7" t="n">
+      <c r="G4" s="8" t="n">
         <v>42372.375</v>
       </c>
-      <c r="H4" s="7" t="n">
+      <c r="H4" s="8" t="n">
         <v>42372.38125</v>
       </c>
       <c r="I4" s="0" t="n">
@@ -1602,13 +1675,13 @@
         <v>23</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1619,21 +1692,21 @@
         <v>3243100</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="F5" s="6" t="n">
+        <v>115</v>
+      </c>
+      <c r="F5" s="7" t="n">
         <v>42372</v>
       </c>
-      <c r="G5" s="7" t="n">
+      <c r="G5" s="8" t="n">
         <v>42372.3819444444</v>
       </c>
-      <c r="H5" s="7" t="n">
+      <c r="H5" s="8" t="n">
         <v>42372.3840277778</v>
       </c>
       <c r="I5" s="0" t="n">
@@ -1652,7 +1725,7 @@
         <v>23</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1663,21 +1736,21 @@
         <v>3243600</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="F6" s="6" t="n">
+        <v>115</v>
+      </c>
+      <c r="F6" s="7" t="n">
         <v>42458</v>
       </c>
-      <c r="G6" s="7" t="n">
+      <c r="G6" s="8" t="n">
         <v>42430.3819444445</v>
       </c>
-      <c r="H6" s="7" t="n">
+      <c r="H6" s="8" t="n">
         <v>42430.3888888889</v>
       </c>
       <c r="I6" s="0" t="str">
@@ -1760,22 +1833,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1783,18 +1856,18 @@
         <v>123</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="E2" s="6" t="n">
+        <v>127</v>
+      </c>
+      <c r="E2" s="7" t="n">
         <v>42372</v>
       </c>
-      <c r="F2" s="6" t="n">
+      <c r="F2" s="7" t="n">
         <v>42524</v>
       </c>
     </row>
@@ -1803,19 +1876,19 @@
         <v>789</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D3" s="0" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
-      <c r="E3" s="6" t="n">
+      <c r="E3" s="7" t="n">
         <v>42458</v>
       </c>
-      <c r="F3" s="6" t="n">
+      <c r="F3" s="7" t="n">
         <v>73051</v>
       </c>
     </row>
@@ -1852,44 +1925,44 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="n">
+      <c r="A2" s="9" t="n">
         <v>3243400</v>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="5" t="n">
         <v>42445.375</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>3243100</v>
       </c>
-      <c r="B3" s="6" t="n">
+      <c r="B3" s="7" t="n">
         <v>42372</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BSIS-1556: Add Division sheet to BSIS import spreadsheet
Add division sheet to import spreadsheet. Includes some test data.
</commit_message>
<xml_diff>
--- a/src/test/resources/fixtures/BSIS-import.xlsx
+++ b/src/test/resources/fixtures/BSIS-import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="975" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,414 +13,480 @@
     <sheet name="Donations" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Deferrals" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Outcomes" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Divisions" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="134">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>isUsageSite</t>
-  </si>
-  <si>
-    <t>isMobileSite</t>
-  </si>
-  <si>
-    <t>isVenue</t>
-  </si>
-  <si>
-    <t>isProcessingSite</t>
-  </si>
-  <si>
-    <t>isDistributionSite</t>
-  </si>
-  <si>
-    <t>isTestingSite</t>
-  </si>
-  <si>
-    <t>isDeleted</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>First</t>
-  </si>
-  <si>
-    <t>First Location</t>
-  </si>
-  <si>
-    <t>Second</t>
-  </si>
-  <si>
-    <t>Third</t>
-  </si>
-  <si>
-    <t>Fourth</t>
-  </si>
-  <si>
-    <t>A venue</t>
-  </si>
-  <si>
-    <t>externalDonorId</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>middleName</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>callingName</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>preferredLanguage</t>
-  </si>
-  <si>
-    <t>birthDate</t>
-  </si>
-  <si>
-    <t>bloodAbo</t>
-  </si>
-  <si>
-    <t>bloodRh</t>
-  </si>
-  <si>
-    <t>venue</t>
-  </si>
-  <si>
-    <t>idType</t>
-  </si>
-  <si>
-    <t>idNumber</t>
-  </si>
-  <si>
-    <t>preferredContactType</t>
-  </si>
-  <si>
-    <t>mobileNumber</t>
-  </si>
-  <si>
-    <t>homeNumber</t>
-  </si>
-  <si>
-    <t>workNumber</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>preferredAddressType</t>
-  </si>
-  <si>
-    <t>homeAddressLine1</t>
-  </si>
-  <si>
-    <t>homeAddressLine2</t>
-  </si>
-  <si>
-    <t>homeAddressCity</t>
-  </si>
-  <si>
-    <t>homeAddressProvince</t>
-  </si>
-  <si>
-    <t>homeAddressDistrict</t>
-  </si>
-  <si>
-    <t>homeAddressState</t>
-  </si>
-  <si>
-    <t>homeAddressCountry</t>
-  </si>
-  <si>
-    <t>homeAddressZipcode</t>
-  </si>
-  <si>
-    <t>workAddressLine1</t>
-  </si>
-  <si>
-    <t>workAddressLine2</t>
-  </si>
-  <si>
-    <t>workAddressCity</t>
-  </si>
-  <si>
-    <t>workAddressProvince</t>
-  </si>
-  <si>
-    <t>workAddressDistrict</t>
-  </si>
-  <si>
-    <t>workAddressCountry</t>
-  </si>
-  <si>
-    <t>workAddressState</t>
-  </si>
-  <si>
-    <t>workAddressZipcode</t>
-  </si>
-  <si>
-    <t>postalAddressLine1</t>
-  </si>
-  <si>
-    <t>postalAddressLine2</t>
-  </si>
-  <si>
-    <t>postalAddressCity</t>
-  </si>
-  <si>
-    <t>postalAddressProvince</t>
-  </si>
-  <si>
-    <t>postalAddressDistrict</t>
-  </si>
-  <si>
-    <t>postalAddressCountry</t>
-  </si>
-  <si>
-    <t>postalAddressState</t>
-  </si>
-  <si>
-    <t>postalAddressZipcode</t>
-  </si>
-  <si>
-    <t>Mr</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>Dave</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>Imported Donor</t>
-  </si>
-  <si>
-    <t>National Id</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>0768198075</t>
-  </si>
-  <si>
-    <t>0214615177</t>
-  </si>
-  <si>
-    <t>0217010939</t>
-  </si>
-  <si>
-    <t>dave@email.com</t>
-  </si>
-  <si>
-    <t>Home Address</t>
-  </si>
-  <si>
-    <t>1 Appartment House</t>
-  </si>
-  <si>
-    <t>123 Street</t>
-  </si>
-  <si>
-    <t>Cape Town</t>
-  </si>
-  <si>
-    <t>Western Cape</t>
-  </si>
-  <si>
-    <t>Gardens</t>
-  </si>
-  <si>
-    <t>South Africa</t>
-  </si>
-  <si>
-    <t>Unit D11 Westlake Square</t>
-  </si>
-  <si>
-    <t>Westlake Drive</t>
-  </si>
-  <si>
-    <t>Westlake</t>
-  </si>
-  <si>
-    <t>P.O. Box 12345</t>
-  </si>
-  <si>
-    <t>The Post Office</t>
-  </si>
-  <si>
-    <t>Vlaeberg</t>
-  </si>
-  <si>
-    <t>Mrs</t>
-  </si>
-  <si>
-    <t>Jane</t>
-  </si>
-  <si>
-    <t>Mary</t>
-  </si>
-  <si>
-    <t>Doe</t>
-  </si>
-  <si>
-    <t>Janey</t>
-  </si>
-  <si>
-    <t>female</t>
-  </si>
-  <si>
-    <t>Afrikaans</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>jane@email.com</t>
-  </si>
-  <si>
-    <t>Prof</t>
-  </si>
-  <si>
-    <t>Donald</t>
-  </si>
-  <si>
-    <t>Brown</t>
-  </si>
-  <si>
-    <t>donationIdentificationNumber</t>
-  </si>
-  <si>
-    <t>donationType</t>
-  </si>
-  <si>
-    <t>packType</t>
-  </si>
-  <si>
-    <t>donationDate</t>
-  </si>
-  <si>
-    <t>bleedStartTime</t>
-  </si>
-  <si>
-    <t>bleedEndTime</t>
-  </si>
-  <si>
-    <t>donorWeight</t>
-  </si>
-  <si>
-    <t>bloodPressureSystolic</t>
-  </si>
-  <si>
-    <t>bloodPressureDiastolic</t>
-  </si>
-  <si>
-    <t>donorPulse</t>
-  </si>
-  <si>
-    <t>haemoglobinCount</t>
-  </si>
-  <si>
-    <t>haemoglobinLevel</t>
-  </si>
-  <si>
-    <t>adverseEventType</t>
-  </si>
-  <si>
-    <t>adverseEventComment</t>
-  </si>
-  <si>
-    <t>Voluntary</t>
-  </si>
-  <si>
-    <t>Single</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>Haematoma</t>
-  </si>
-  <si>
-    <t>bla</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>More notes</t>
-  </si>
-  <si>
-    <t>deferralReason</t>
-  </si>
-  <si>
-    <t>deferralReasonText</t>
-  </si>
-  <si>
-    <t>createdDate</t>
-  </si>
-  <si>
-    <t>deferredUntil</t>
-  </si>
-  <si>
-    <t>Other reasons</t>
-  </si>
-  <si>
-    <t>Had nausea</t>
-  </si>
-  <si>
-    <t>testedOn</t>
-  </si>
-  <si>
-    <t>bloodTestName</t>
-  </si>
-  <si>
-    <t>outcome</t>
-  </si>
-  <si>
-    <t>HIV</t>
-  </si>
-  <si>
-    <t>POS</t>
-  </si>
-  <si>
-    <t>NEG</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="154">
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isUsageSite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isMobileSite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isVenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isProcessingSite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isDistributionSite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isTestingSite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isDeleted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Third</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fourth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A venue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">externalDonorId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">middleName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">callingName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preferredLanguage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">birthDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bloodAbo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bloodRh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">venue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preferredContactType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mobileNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preferredAddressType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressLine1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressLine2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressCity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressProvince</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressDistrict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressCountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homeAddressZipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressLine1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressLine2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressCity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressProvince</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressDistrict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressCountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workAddressZipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressLine1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressLine2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressCity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressProvince</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressDistrict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressCountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postalAddressZipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imported Donor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">National Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0768198075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0214615177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0217010939</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dave@email.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Appartment House</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123 Street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cape Town</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Cape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gardens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Africa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit D11 Westlake Square</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Westlake Drive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Westlake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P.O. Box 12345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Post Office</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vlaeberg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Janey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Afrikaans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jane@email.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prof</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Donald</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donationIdentificationNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donationType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">packType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donationDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bleedStartTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bleedEndTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donorWeight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bloodPressureSystolic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bloodPressureDiastolic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donorPulse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">haemoglobinCount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">haemoglobinLevel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adverseEventType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adverseEventComment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haematoma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deferralReason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deferralReasonText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">createdDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deferredUntil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other reasons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Had nausea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testedOn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bloodTestName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">outcome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HIV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">province1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov1-municipality1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov1-mun1-ward1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov1-mun1-ward2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov1-mun1-ward3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov1-mun1-ward4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov1-mun1-ward5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov1-municipality2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov1-mun2-ward1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov1-mun2-ward2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov1-mun2-ward3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">province2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov2-municipality1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov2-mun2-ward1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov2-mun2-ward2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov2-mun2-ward3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov2-mun2-ward4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov2-mun2-ward5</t>
   </si>
 </sst>
 </file>
@@ -428,7 +494,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
     <numFmt numFmtId="166" formatCode="YY/MM/DD\ HH:MM"/>
   </numFmts>
@@ -504,16 +570,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -564,22 +626,22 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.5765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6785714285714"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="55.3469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="54.1326530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.1530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -627,15 +689,15 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -659,19 +721,19 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -692,19 +754,19 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="G4" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -729,15 +791,15 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G5" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -779,52 +841,52 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="3" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.1887755102041"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -861,7 +923,7 @@
       <c r="K1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -991,7 +1053,7 @@
       <c r="H2" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="5" t="n">
+      <c r="I2" s="4" t="n">
         <v>30288</v>
       </c>
       <c r="J2" s="0" t="s">
@@ -1000,7 +1062,7 @@
       <c r="K2" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>68</v>
       </c>
       <c r="M2" s="0" t="s">
@@ -1054,10 +1116,10 @@
       <c r="AC2" s="0" t="n">
         <v>8001</v>
       </c>
-      <c r="AD2" s="6" t="s">
+      <c r="AD2" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AE2" s="6" t="s">
+      <c r="AE2" s="5" t="s">
         <v>83</v>
       </c>
       <c r="AF2" s="0" t="s">
@@ -1128,7 +1190,7 @@
       <c r="H3" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="I3" s="5" t="n">
+      <c r="I3" s="4" t="n">
         <v>26575</v>
       </c>
       <c r="J3" s="0" t="s">
@@ -1137,7 +1199,7 @@
       <c r="K3" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>68</v>
       </c>
       <c r="M3" s="0" t="s">
@@ -1191,10 +1253,10 @@
       <c r="AC3" s="0" t="n">
         <v>8001</v>
       </c>
-      <c r="AD3" s="6" t="s">
+      <c r="AD3" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AE3" s="6" t="s">
+      <c r="AE3" s="5" t="s">
         <v>83</v>
       </c>
       <c r="AF3" s="0" t="s">
@@ -1267,7 +1329,7 @@
       <c r="H4" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="I4" s="7" t="n">
+      <c r="I4" s="6" t="n">
         <v>36443</v>
       </c>
       <c r="J4" s="0" t="str">
@@ -1435,26 +1497,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8316326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1532,13 +1590,13 @@
       <c r="E2" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="F2" s="7" t="n">
+      <c r="F2" s="6" t="n">
         <v>42432.0833333333</v>
       </c>
-      <c r="G2" s="8" t="n">
+      <c r="G2" s="7" t="n">
         <v>42432.375</v>
       </c>
-      <c r="H2" s="8" t="n">
+      <c r="H2" s="7" t="n">
         <v>42432.38125</v>
       </c>
       <c r="I2" s="0" t="n">
@@ -1591,13 +1649,13 @@
       <c r="E3" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="F3" s="7" t="n">
+      <c r="F3" s="6" t="n">
         <v>42432.5</v>
       </c>
-      <c r="G3" s="8" t="n">
+      <c r="G3" s="7" t="n">
         <v>42432.3819444444</v>
       </c>
-      <c r="H3" s="8" t="n">
+      <c r="H3" s="7" t="n">
         <v>42432.3840277778</v>
       </c>
       <c r="I3" s="0" t="n">
@@ -1650,13 +1708,13 @@
       <c r="E4" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="F4" s="7" t="n">
+      <c r="F4" s="6" t="n">
         <v>42372</v>
       </c>
-      <c r="G4" s="8" t="n">
+      <c r="G4" s="7" t="n">
         <v>42372.375</v>
       </c>
-      <c r="H4" s="8" t="n">
+      <c r="H4" s="7" t="n">
         <v>42372.38125</v>
       </c>
       <c r="I4" s="0" t="n">
@@ -1700,13 +1758,13 @@
       <c r="E5" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="F5" s="7" t="n">
+      <c r="F5" s="6" t="n">
         <v>42372</v>
       </c>
-      <c r="G5" s="8" t="n">
+      <c r="G5" s="7" t="n">
         <v>42372.3819444444</v>
       </c>
-      <c r="H5" s="8" t="n">
+      <c r="H5" s="7" t="n">
         <v>42372.3840277778</v>
       </c>
       <c r="I5" s="0" t="n">
@@ -1744,13 +1802,13 @@
       <c r="E6" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="F6" s="7" t="n">
+      <c r="F6" s="6" t="n">
         <v>42458</v>
       </c>
-      <c r="G6" s="8" t="n">
+      <c r="G6" s="7" t="n">
         <v>42430.3819444445</v>
       </c>
-      <c r="H6" s="8" t="n">
+      <c r="H6" s="7" t="n">
         <v>42430.3888888889</v>
       </c>
       <c r="I6" s="0" t="str">
@@ -1822,13 +1880,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1864,10 +1922,10 @@
       <c r="D2" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="E2" s="7" t="n">
+      <c r="E2" s="6" t="n">
         <v>42372</v>
       </c>
-      <c r="F2" s="7" t="n">
+      <c r="F2" s="6" t="n">
         <v>42524</v>
       </c>
     </row>
@@ -1885,10 +1943,10 @@
         <f aca="false">""</f>
         <v/>
       </c>
-      <c r="E3" s="7" t="n">
+      <c r="E3" s="6" t="n">
         <v>42458</v>
       </c>
-      <c r="F3" s="7" t="n">
+      <c r="F3" s="6" t="n">
         <v>73051</v>
       </c>
     </row>
@@ -1916,11 +1974,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1938,10 +1995,10 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="n">
+      <c r="A2" s="8" t="n">
         <v>3243400</v>
       </c>
-      <c r="B2" s="5" t="n">
+      <c r="B2" s="4" t="n">
         <v>42445.375</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -1955,7 +2012,7 @@
       <c r="A3" s="0" t="n">
         <v>3243100</v>
       </c>
-      <c r="B3" s="7" t="n">
+      <c r="B3" s="6" t="n">
         <v>42372</v>
       </c>
       <c r="C3" s="0" t="s">
@@ -1974,4 +2031,242 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B1:D1" type="none">
+      <formula1>booleans</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
BSIS-1556: Update to division test data in Import spreadsheet
Update to division test data in import spreadsheet.
</commit_message>
<xml_diff>
--- a/src/test/resources/fixtures/BSIS-import.xlsx
+++ b/src/test/resources/fixtures/BSIS-import.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="145">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -447,46 +447,19 @@
     <t xml:space="preserve">prov1-mun1-ward2</t>
   </si>
   <si>
-    <t xml:space="preserve">prov1-mun1-ward3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prov1-mun1-ward4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prov1-mun1-ward5</t>
-  </si>
-  <si>
     <t xml:space="preserve">prov1-municipality2</t>
   </si>
   <si>
     <t xml:space="preserve">prov1-mun2-ward1</t>
   </si>
   <si>
-    <t xml:space="preserve">prov1-mun2-ward2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prov1-mun2-ward3</t>
+    <t xml:space="preserve">prov2-mun2-ward1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov2-municipality1</t>
   </si>
   <si>
     <t xml:space="preserve">province2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prov2-municipality1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prov2-mun2-ward1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prov2-mun2-ward2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prov2-mun2-ward3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prov2-mun2-ward4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prov2-mun2-ward5</t>
   </si>
 </sst>
 </file>
@@ -627,7 +600,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -835,7 +808,7 @@
   </sheetPr>
   <dimension ref="1:4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AD1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1492,7 +1465,7 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2038,10 +2011,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2108,10 +2081,10 @@
         <v>140</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2122,7 +2095,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2133,7 +2106,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2144,7 +2117,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2152,106 +2125,7 @@
         <v>144</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="B13" s="0" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="B18" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="B19" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BSIS-1556: Update test data in BSIS-import.xlsx Divisions sheet
Simplify divisions defined in Divisions sheet. Parents are now all before
their children. Division sheet also moved to first position.
</commit_message>
<xml_diff>
--- a/src/test/resources/fixtures/BSIS-import.xlsx
+++ b/src/test/resources/fixtures/BSIS-import.xlsx
@@ -5,15 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Locations" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Donors" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Donations" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Deferrals" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Outcomes" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Divisions" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Divisions" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Locations" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Donors" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Donations" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Deferrals" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Outcomes" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -30,6 +30,39 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
+    <t xml:space="preserve">level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">province1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov1-municipality1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov1-mun1-ward1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov1-mun1-ward2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov1-municipality2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov1-mun2-ward1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">province2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov2-municipality1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prov2-mun2-ward1</t>
+  </si>
+  <si>
     <t xml:space="preserve">isUsageSite</t>
   </si>
   <si>
@@ -427,39 +460,6 @@
   </si>
   <si>
     <t xml:space="preserve">NEG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">province1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prov1-municipality1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prov1-mun1-ward1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prov1-mun1-ward2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prov1-municipality2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prov1-mun2-ward1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prov2-mun2-ward1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prov2-municipality1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">province2</t>
   </si>
 </sst>
 </file>
@@ -597,6 +597,144 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9744897959184"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B1:D1" type="none">
+      <formula1>booleans</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -605,16 +743,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="54.1326530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="53.4591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -622,33 +759,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B2" s="0" t="n">
         <f aca="false">FALSE()</f>
@@ -679,12 +816,12 @@
         <v>0</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">FALSE()</f>
@@ -717,7 +854,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">TRUE()</f>
@@ -750,7 +887,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B5" s="0" t="n">
         <f aca="false">FALSE()</f>
@@ -781,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -801,7 +938,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -814,189 +951,188 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
@@ -1006,133 +1142,133 @@
         <v>123</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="I2" s="4" t="n">
         <v>30288</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="O2" s="0" t="n">
         <v>8212030162083</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="Z2" s="0" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AB2" s="0" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AC2" s="0" t="n">
         <v>8001</v>
       </c>
       <c r="AD2" s="5" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="AE2" s="5" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="AF2" s="0" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="AG2" s="0" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AH2" s="0" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="AI2" s="0" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AJ2" s="0" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AK2" s="0" t="n">
         <v>8001</v>
       </c>
       <c r="AL2" s="0" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="AM2" s="0" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="AN2" s="0" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="AO2" s="0" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AP2" s="0" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="AQ2" s="0" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AR2" s="0" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AS2" s="0" t="n">
         <v>8018</v>
@@ -1143,133 +1279,133 @@
         <v>456</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="I3" s="4" t="n">
         <v>26575</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="O3" s="0" t="n">
         <v>7210030162086</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="Y3" s="0" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="Z3" s="0" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="AA3" s="0" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AB3" s="0" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AC3" s="0" t="n">
         <v>8001</v>
       </c>
       <c r="AD3" s="5" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="AE3" s="5" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="AF3" s="0" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="AG3" s="0" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AH3" s="0" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="AI3" s="0" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AJ3" s="0" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AK3" s="0" t="n">
         <v>8001</v>
       </c>
       <c r="AL3" s="0" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="AM3" s="0" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="AN3" s="0" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="AO3" s="0" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AP3" s="0" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="AQ3" s="0" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AR3" s="0" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AS3" s="0" t="n">
         <v>8018</v>
@@ -1280,27 +1416,27 @@
         <v>789</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="D4" s="0" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
       <c r="E4" s="0" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="F4" s="0" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
       <c r="G4" s="0" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="I4" s="6" t="n">
         <v>36443</v>
@@ -1315,7 +1451,7 @@
       </c>
       <c r="L4" s="0"/>
       <c r="M4" s="0" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="N4" s="0" t="str">
         <f aca="false">""</f>
@@ -1442,389 +1578,6 @@
         <v/>
       </c>
       <c r="AS4" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:S6"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.1224489795918"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>123</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>3243400</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="F2" s="6" t="n">
-        <v>42432.0833333333</v>
-      </c>
-      <c r="G2" s="7" t="n">
-        <v>42432.375</v>
-      </c>
-      <c r="H2" s="7" t="n">
-        <v>42432.38125</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>89</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>113</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>56</v>
-      </c>
-      <c r="L2" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="M2" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="R2" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="S2" s="0" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>456</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>3243500</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="F3" s="6" t="n">
-        <v>42432.5</v>
-      </c>
-      <c r="G3" s="7" t="n">
-        <v>42432.3819444444</v>
-      </c>
-      <c r="H3" s="7" t="n">
-        <v>42432.3840277778</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>75</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="M3" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="O3" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="P3" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q3" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="R3" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="S3" s="0" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>123</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>3243200</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="F4" s="6" t="n">
-        <v>42372</v>
-      </c>
-      <c r="G4" s="7" t="n">
-        <v>42372.375</v>
-      </c>
-      <c r="H4" s="7" t="n">
-        <v>42372.38125</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>89</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>113</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <v>56</v>
-      </c>
-      <c r="L4" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="M4" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="N4" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q4" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="R4" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>456</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>3243100</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="F5" s="6" t="n">
-        <v>42372</v>
-      </c>
-      <c r="G5" s="7" t="n">
-        <v>42372.3819444444</v>
-      </c>
-      <c r="H5" s="7" t="n">
-        <v>42372.3840277778</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>75</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K5" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="L5" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="M5" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="N5" s="0" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>789</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>3243600</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="F6" s="6" t="n">
-        <v>42458</v>
-      </c>
-      <c r="G6" s="7" t="n">
-        <v>42430.3819444445</v>
-      </c>
-      <c r="H6" s="7" t="n">
-        <v>42430.3888888889</v>
-      </c>
-      <c r="I6" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="J6" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="K6" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="L6" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="M6" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="N6" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="O6" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="P6" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="Q6" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="R6" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="S6" s="0" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
@@ -1845,88 +1598,381 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>111</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>125</v>
+      <c r="Q1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>123</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>9</v>
+      <c r="B2" s="0" t="n">
+        <v>3243400</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="F2" s="6" t="n">
+        <v>42432.0833333333</v>
+      </c>
+      <c r="G2" s="7" t="n">
+        <v>42432.375</v>
+      </c>
+      <c r="H2" s="7" t="n">
+        <v>42432.38125</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="N2" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="E2" s="6" t="n">
-        <v>42372</v>
-      </c>
-      <c r="F2" s="6" t="n">
-        <v>42524</v>
+      <c r="O2" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
+        <v>456</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>3243500</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3" s="6" t="n">
+        <v>42432.5</v>
+      </c>
+      <c r="G3" s="7" t="n">
+        <v>42432.3819444444</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>42432.3840277778</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>3243200</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4" s="6" t="n">
+        <v>42372</v>
+      </c>
+      <c r="G4" s="7" t="n">
+        <v>42372.375</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>42372.38125</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>456</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>3243100</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>42372</v>
+      </c>
+      <c r="G5" s="7" t="n">
+        <v>42372.3819444444</v>
+      </c>
+      <c r="H5" s="7" t="n">
+        <v>42372.3840277778</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
         <v>789</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="B6" s="0" t="n">
+        <v>3243600</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="D3" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="E3" s="6" t="n">
+      <c r="F6" s="6" t="n">
         <v>42458</v>
       </c>
-      <c r="F3" s="6" t="n">
-        <v>73051</v>
+      <c r="G6" s="7" t="n">
+        <v>42430.3819444445</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>42430.3888888889</v>
+      </c>
+      <c r="I6" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="J6" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="K6" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="L6" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="M6" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="N6" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="O6" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="P6" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="Q6" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="R6" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="S6" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1939,66 +1985,87 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>128</v>
+        <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="n">
-        <v>3243400</v>
-      </c>
-      <c r="B2" s="4" t="n">
-        <v>42445.375</v>
+      <c r="A2" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>20</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>132</v>
+        <v>138</v>
+      </c>
+      <c r="E2" s="6" t="n">
+        <v>42372</v>
+      </c>
+      <c r="F2" s="6" t="n">
+        <v>42524</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>3243100</v>
-      </c>
-      <c r="B3" s="6" t="n">
-        <v>42372</v>
+        <v>789</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>20</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
+      </c>
+      <c r="D3" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="E3" s="6" t="n">
+        <v>42458</v>
+      </c>
+      <c r="F3" s="6" t="n">
+        <v>73051</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2011,133 +2078,67 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="1"/>
+        <v>140</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>1</v>
+      <c r="A2" s="8" t="n">
+        <v>3243400</v>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>42445.375</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>2</v>
+      <c r="A3" s="0" t="n">
+        <v>3243100</v>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>42372</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="B8" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B1:D1" type="none">
-      <formula1>booleans</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
BSIS-1556: Improve names of divisions
Use real world division names to make the test data easier to understand.
</commit_message>
<xml_diff>
--- a/src/test/resources/fixtures/BSIS-import.xlsx
+++ b/src/test/resources/fixtures/BSIS-import.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="144">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -36,31 +36,31 @@
     <t xml:space="preserve">parent</t>
   </si>
   <si>
-    <t xml:space="preserve">province1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prov1-municipality1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prov1-mun1-ward1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prov1-mun1-ward2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prov1-municipality2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prov1-mun2-ward1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">province2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prov2-municipality1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prov2-mun2-ward1</t>
+    <t xml:space="preserve">Western Cape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City of Cape Town</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khayelitsha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mitchell’s Plain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cape Winelands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stellenbosch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gauteng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tshwane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pretoria</t>
   </si>
   <si>
     <t xml:space="preserve">isUsageSite</t>
@@ -295,9 +295,6 @@
   </si>
   <si>
     <t xml:space="preserve">Cape Town</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Western Cape</t>
   </si>
   <si>
     <t xml:space="preserve">Gardens</t>
@@ -600,12 +597,13 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -743,15 +741,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="53.4591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="52.780612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -951,51 +950,47 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="17.280612244898"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1211,64 +1206,64 @@
         <v>89</v>
       </c>
       <c r="Y2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z2" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="Z2" s="0" t="s">
+      <c r="AA2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB2" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="AA2" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB2" s="0" t="s">
-        <v>92</v>
       </c>
       <c r="AC2" s="0" t="n">
         <v>8001</v>
       </c>
       <c r="AD2" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AE2" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="AE2" s="5" t="s">
+      <c r="AF2" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="AF2" s="0" t="s">
-        <v>95</v>
-      </c>
       <c r="AG2" s="0" t="s">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="AH2" s="0" t="s">
         <v>89</v>
       </c>
       <c r="AI2" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AJ2" s="0" t="s">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="AK2" s="0" t="n">
         <v>8001</v>
       </c>
       <c r="AL2" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="AM2" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="AM2" s="0" t="s">
+      <c r="AN2" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="AN2" s="0" t="s">
-        <v>98</v>
-      </c>
       <c r="AO2" s="0" t="s">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="AP2" s="0" t="s">
         <v>89</v>
       </c>
       <c r="AQ2" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AR2" s="0" t="s">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="AS2" s="0" t="n">
         <v>8018</v>
@@ -1279,31 +1274,31 @@
         <v>456</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>104</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>105</v>
       </c>
       <c r="I3" s="4" t="n">
         <v>26575</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K3" s="0" t="s">
         <v>78</v>
@@ -1333,7 +1328,7 @@
         <v>84</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="U3" s="0" t="s">
         <v>86</v>
@@ -1348,64 +1343,64 @@
         <v>89</v>
       </c>
       <c r="Y3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z3" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="Z3" s="0" t="s">
+      <c r="AA3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB3" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="AA3" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB3" s="0" t="s">
-        <v>92</v>
       </c>
       <c r="AC3" s="0" t="n">
         <v>8001</v>
       </c>
       <c r="AD3" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AE3" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="AE3" s="5" t="s">
+      <c r="AF3" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="AF3" s="0" t="s">
-        <v>95</v>
-      </c>
       <c r="AG3" s="0" t="s">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="AH3" s="0" t="s">
         <v>89</v>
       </c>
       <c r="AI3" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AJ3" s="0" t="s">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="AK3" s="0" t="n">
         <v>8001</v>
       </c>
       <c r="AL3" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="AM3" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="AM3" s="0" t="s">
+      <c r="AN3" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="AN3" s="0" t="s">
-        <v>98</v>
-      </c>
       <c r="AO3" s="0" t="s">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="AP3" s="0" t="s">
         <v>89</v>
       </c>
       <c r="AQ3" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AR3" s="0" t="s">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="AS3" s="0" t="n">
         <v>8018</v>
@@ -1416,17 +1411,17 @@
         <v>789</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="str">
+        <f aca="false">""</f>
+        <v/>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="D4" s="0" t="str">
-        <f aca="false">""</f>
-        <v/>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>110</v>
       </c>
       <c r="F4" s="0" t="str">
         <f aca="false">""</f>
@@ -1606,26 +1601,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1633,49 +1628,49 @@
         <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>35</v>
@@ -1698,10 +1693,10 @@
         <v>20</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>126</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>42432.0833333333</v>
@@ -1728,22 +1723,22 @@
         <v>23</v>
       </c>
       <c r="N2" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="O2" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="P2" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="Q2" s="0" t="s">
         <v>129</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>130</v>
       </c>
       <c r="R2" s="0" t="s">
         <v>78</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1757,10 +1752,10 @@
         <v>20</v>
       </c>
       <c r="D3" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>126</v>
       </c>
       <c r="F3" s="6" t="n">
         <v>42432.5</v>
@@ -1787,13 +1782,13 @@
         <v>23</v>
       </c>
       <c r="N3" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="O3" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="O3" s="0" t="s">
+      <c r="P3" s="0" t="s">
         <v>128</v>
-      </c>
-      <c r="P3" s="0" t="s">
-        <v>129</v>
       </c>
       <c r="Q3" s="0" t="s">
         <v>77</v>
@@ -1802,7 +1797,7 @@
         <v>78</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1816,10 +1811,10 @@
         <v>20</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>126</v>
       </c>
       <c r="F4" s="6" t="n">
         <v>42372</v>
@@ -1846,10 +1841,10 @@
         <v>23</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="R4" s="0" t="s">
         <v>78</v>
@@ -1866,10 +1861,10 @@
         <v>24</v>
       </c>
       <c r="D5" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>126</v>
       </c>
       <c r="F5" s="6" t="n">
         <v>42372</v>
@@ -1896,7 +1891,7 @@
         <v>23</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1910,10 +1905,10 @@
         <v>20</v>
       </c>
       <c r="D6" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>126</v>
       </c>
       <c r="F6" s="6" t="n">
         <v>42458</v>
@@ -1993,12 +1988,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2009,16 +2005,16 @@
         <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2029,10 +2025,10 @@
         <v>20</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>137</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>138</v>
       </c>
       <c r="E2" s="6" t="n">
         <v>42372</v>
@@ -2049,7 +2045,7 @@
         <v>20</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D3" s="0" t="str">
         <f aca="false">""</f>
@@ -2086,25 +2082,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2115,10 +2110,10 @@
         <v>42445.375</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>142</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2129,10 +2124,10 @@
         <v>42372</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BSIS-1634 Add divisionLevel3 to location import sheet
Populate divisions when importing locations from the spreadsheet using
the data importer.
</commit_message>
<xml_diff>
--- a/src/test/resources/fixtures/BSIS-import.xlsx
+++ b/src/test/resources/fixtures/BSIS-import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Divisions" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="145">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t xml:space="preserve">notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">divisionLevel3</t>
   </si>
   <si>
     <t xml:space="preserve">First</t>
@@ -596,14 +599,14 @@
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -733,24 +736,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J19" activeCellId="0" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="52.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="52.1071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -781,10 +784,13 @@
       <c r="I1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" s="0" t="n">
         <f aca="false">FALSE()</f>
@@ -815,12 +821,15 @@
         <v>0</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">FALSE()</f>
@@ -850,10 +859,13 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="J3" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">TRUE()</f>
@@ -883,10 +895,13 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="J4" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="0" t="n">
         <f aca="false">FALSE()</f>
@@ -917,7 +932,10 @@
         <v>0</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -950,184 +968,189 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>19</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
@@ -1137,106 +1160,106 @@
         <v>123</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I2" s="4" t="n">
         <v>30288</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="O2" s="0" t="n">
         <v>8212030162083</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Y2" s="0" t="s">
         <v>3</v>
       </c>
       <c r="Z2" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AA2" s="0" t="s">
         <v>3</v>
       </c>
       <c r="AB2" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AC2" s="0" t="n">
         <v>8001</v>
       </c>
       <c r="AD2" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AE2" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AF2" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AG2" s="0" t="s">
         <v>3</v>
       </c>
       <c r="AH2" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AI2" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AJ2" s="0" t="s">
         <v>3</v>
@@ -1245,22 +1268,22 @@
         <v>8001</v>
       </c>
       <c r="AL2" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AM2" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AN2" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AO2" s="0" t="s">
         <v>3</v>
       </c>
       <c r="AP2" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AQ2" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AR2" s="0" t="s">
         <v>3</v>
@@ -1274,106 +1297,106 @@
         <v>456</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I3" s="4" t="n">
         <v>26575</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="O3" s="0" t="n">
         <v>7210030162086</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Y3" s="0" t="s">
         <v>3</v>
       </c>
       <c r="Z3" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AA3" s="0" t="s">
         <v>3</v>
       </c>
       <c r="AB3" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AC3" s="0" t="n">
         <v>8001</v>
       </c>
       <c r="AD3" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AE3" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AF3" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AG3" s="0" t="s">
         <v>3</v>
       </c>
       <c r="AH3" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AI3" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AJ3" s="0" t="s">
         <v>3</v>
@@ -1382,22 +1405,22 @@
         <v>8001</v>
       </c>
       <c r="AL3" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AM3" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AN3" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AO3" s="0" t="s">
         <v>3</v>
       </c>
       <c r="AP3" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AQ3" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AR3" s="0" t="s">
         <v>3</v>
@@ -1411,27 +1434,27 @@
         <v>789</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D4" s="0" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
       <c r="E4" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F4" s="0" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
       <c r="G4" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I4" s="6" t="n">
         <v>36443</v>
@@ -1446,7 +1469,7 @@
       </c>
       <c r="L4" s="0"/>
       <c r="M4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N4" s="0" t="str">
         <f aca="false">""</f>
@@ -1601,82 +1624,82 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>19</v>
@@ -1690,13 +1713,13 @@
         <v>3243400</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>42432.0833333333</v>
@@ -1723,22 +1746,22 @@
         <v>23</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1749,13 +1772,13 @@
         <v>3243500</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F3" s="6" t="n">
         <v>42432.5</v>
@@ -1782,22 +1805,22 @@
         <v>23</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1808,13 +1831,13 @@
         <v>3243200</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F4" s="6" t="n">
         <v>42372</v>
@@ -1841,13 +1864,13 @@
         <v>23</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1858,13 +1881,13 @@
         <v>3243100</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F5" s="6" t="n">
         <v>42372</v>
@@ -1891,7 +1914,7 @@
         <v>23</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1902,13 +1925,13 @@
         <v>3243600</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F6" s="6" t="n">
         <v>42458</v>
@@ -1988,33 +2011,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2022,13 +2045,13 @@
         <v>123</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E2" s="6" t="n">
         <v>42372</v>
@@ -2042,10 +2065,10 @@
         <v>789</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D3" s="0" t="str">
         <f aca="false">""</f>
@@ -2082,24 +2105,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2110,10 +2134,10 @@
         <v>42445.375</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2124,10 +2148,10 @@
         <v>42372</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BSIS-2574 Add isReferralSite to DataImportService * A new site referral site was added to locations. The DataImport and the excel spread sheet had to be updated as well.
</commit_message>
<xml_diff>
--- a/src/test/resources/fixtures/BSIS-import.xlsx
+++ b/src/test/resources/fixtures/BSIS-import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Divisions" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="146">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t xml:space="preserve">isTestingSite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isReferralSite</t>
   </si>
   <si>
     <t xml:space="preserve">isDeleted</t>
@@ -543,12 +546,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -573,10 +584,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -605,8 +612,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -736,24 +742,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J19" activeCellId="0" sqref="J19"/>
+      <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="52.1071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.0663265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -787,10 +793,13 @@
       <c r="J1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" s="0" t="n">
         <f aca="false">FALSE()</f>
@@ -820,16 +829,20 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="0" t="s">
+      <c r="I2" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">FALSE()</f>
@@ -855,17 +868,21 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="K3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">TRUE()</f>
@@ -891,17 +908,21 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="2" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="K4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" s="0" t="n">
         <f aca="false">FALSE()</f>
@@ -931,10 +952,14 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I5" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" s="0" t="s">
+      <c r="I5" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -968,189 +993,188 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="4" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>19</v>
+        <v>38</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
@@ -1160,106 +1184,106 @@
         <v>123</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="I2" s="4" t="n">
+        <v>78</v>
+      </c>
+      <c r="I2" s="6" t="n">
         <v>30288</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="L2" s="5" t="s">
         <v>80</v>
       </c>
+      <c r="L2" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="M2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O2" s="0" t="n">
         <v>8212030162083</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="Y2" s="0" t="s">
         <v>3</v>
       </c>
       <c r="Z2" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AA2" s="0" t="s">
         <v>3</v>
       </c>
       <c r="AB2" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AC2" s="0" t="n">
         <v>8001</v>
       </c>
-      <c r="AD2" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="AE2" s="5" t="s">
+      <c r="AD2" s="7" t="s">
         <v>94</v>
       </c>
+      <c r="AE2" s="7" t="s">
+        <v>95</v>
+      </c>
       <c r="AF2" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AG2" s="0" t="s">
         <v>3</v>
       </c>
       <c r="AH2" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AI2" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AJ2" s="0" t="s">
         <v>3</v>
@@ -1268,22 +1292,22 @@
         <v>8001</v>
       </c>
       <c r="AL2" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AM2" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AN2" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AO2" s="0" t="s">
         <v>3</v>
       </c>
       <c r="AP2" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AQ2" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AR2" s="0" t="s">
         <v>3</v>
@@ -1297,106 +1321,106 @@
         <v>456</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="I3" s="4" t="n">
+        <v>106</v>
+      </c>
+      <c r="I3" s="6" t="n">
         <v>26575</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="L3" s="5" t="s">
         <v>80</v>
       </c>
+      <c r="L3" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="M3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O3" s="0" t="n">
         <v>7210030162086</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="Y3" s="0" t="s">
         <v>3</v>
       </c>
       <c r="Z3" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AA3" s="0" t="s">
         <v>3</v>
       </c>
       <c r="AB3" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AC3" s="0" t="n">
         <v>8001</v>
       </c>
-      <c r="AD3" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="AE3" s="5" t="s">
+      <c r="AD3" s="7" t="s">
         <v>94</v>
       </c>
+      <c r="AE3" s="7" t="s">
+        <v>95</v>
+      </c>
       <c r="AF3" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AG3" s="0" t="s">
         <v>3</v>
       </c>
       <c r="AH3" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AI3" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AJ3" s="0" t="s">
         <v>3</v>
@@ -1405,22 +1429,22 @@
         <v>8001</v>
       </c>
       <c r="AL3" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AM3" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AN3" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AO3" s="0" t="s">
         <v>3</v>
       </c>
       <c r="AP3" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AQ3" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AR3" s="0" t="s">
         <v>3</v>
@@ -1434,29 +1458,29 @@
         <v>789</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D4" s="0" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
       <c r="E4" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F4" s="0" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
       <c r="G4" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="I4" s="6" t="n">
+        <v>78</v>
+      </c>
+      <c r="I4" s="8" t="n">
         <v>36443</v>
       </c>
       <c r="J4" s="0" t="str">
@@ -1469,7 +1493,7 @@
       </c>
       <c r="L4" s="0"/>
       <c r="M4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N4" s="0" t="str">
         <f aca="false">""</f>
@@ -1624,85 +1648,85 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="S1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1713,21 +1737,21 @@
         <v>3243400</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="F2" s="6" t="n">
+        <v>127</v>
+      </c>
+      <c r="F2" s="8" t="n">
         <v>42432.0833333333</v>
       </c>
-      <c r="G2" s="7" t="n">
+      <c r="G2" s="9" t="n">
         <v>42432.375</v>
       </c>
-      <c r="H2" s="7" t="n">
+      <c r="H2" s="9" t="n">
         <v>42432.38125</v>
       </c>
       <c r="I2" s="0" t="n">
@@ -1746,22 +1770,22 @@
         <v>23</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1772,21 +1796,21 @@
         <v>3243500</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="F3" s="6" t="n">
+        <v>127</v>
+      </c>
+      <c r="F3" s="8" t="n">
         <v>42432.5</v>
       </c>
-      <c r="G3" s="7" t="n">
+      <c r="G3" s="9" t="n">
         <v>42432.3819444444</v>
       </c>
-      <c r="H3" s="7" t="n">
+      <c r="H3" s="9" t="n">
         <v>42432.3840277778</v>
       </c>
       <c r="I3" s="0" t="n">
@@ -1805,22 +1829,22 @@
         <v>23</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1831,21 +1855,21 @@
         <v>3243200</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="F4" s="6" t="n">
+        <v>127</v>
+      </c>
+      <c r="F4" s="8" t="n">
         <v>42372</v>
       </c>
-      <c r="G4" s="7" t="n">
+      <c r="G4" s="9" t="n">
         <v>42372.375</v>
       </c>
-      <c r="H4" s="7" t="n">
+      <c r="H4" s="9" t="n">
         <v>42372.38125</v>
       </c>
       <c r="I4" s="0" t="n">
@@ -1864,13 +1888,13 @@
         <v>23</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1881,21 +1905,21 @@
         <v>3243100</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="F5" s="6" t="n">
+        <v>127</v>
+      </c>
+      <c r="F5" s="8" t="n">
         <v>42372</v>
       </c>
-      <c r="G5" s="7" t="n">
+      <c r="G5" s="9" t="n">
         <v>42372.3819444444</v>
       </c>
-      <c r="H5" s="7" t="n">
+      <c r="H5" s="9" t="n">
         <v>42372.3840277778</v>
       </c>
       <c r="I5" s="0" t="n">
@@ -1914,7 +1938,7 @@
         <v>23</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1925,21 +1949,21 @@
         <v>3243600</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="F6" s="6" t="n">
+        <v>127</v>
+      </c>
+      <c r="F6" s="8" t="n">
         <v>42458</v>
       </c>
-      <c r="G6" s="7" t="n">
+      <c r="G6" s="9" t="n">
         <v>42430.3819444445</v>
       </c>
-      <c r="H6" s="7" t="n">
+      <c r="H6" s="9" t="n">
         <v>42430.3888888889</v>
       </c>
       <c r="I6" s="0" t="str">
@@ -2011,33 +2035,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2045,18 +2068,18 @@
         <v>123</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="E2" s="6" t="n">
+        <v>139</v>
+      </c>
+      <c r="E2" s="8" t="n">
         <v>42372</v>
       </c>
-      <c r="F2" s="6" t="n">
+      <c r="F2" s="8" t="n">
         <v>42524</v>
       </c>
     </row>
@@ -2065,19 +2088,19 @@
         <v>789</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D3" s="0" t="str">
         <f aca="false">""</f>
         <v/>
       </c>
-      <c r="E3" s="6" t="n">
+      <c r="E3" s="8" t="n">
         <v>42458</v>
       </c>
-      <c r="F3" s="6" t="n">
+      <c r="F3" s="8" t="n">
         <v>73051</v>
       </c>
     </row>
@@ -2105,53 +2128,53 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="n">
+      <c r="A2" s="3" t="n">
         <v>3243400</v>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="6" t="n">
         <v>42445.375</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>3243100</v>
       </c>
-      <c r="B3" s="6" t="n">
+      <c r="B3" s="8" t="n">
         <v>42372</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>